<commit_message>
finish modifying wild encounter insertion script
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -1636,7 +1636,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1939,6 +1939,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -1951,6 +1954,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>20</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -1963,6 +1969,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>20</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -2003,9 +2012,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>20</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -2032,9 +2038,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>20</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -2060,11 +2063,6 @@
       </c>
       <c r="P30">
         <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2474,7 +2472,7 @@
 
 <file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2888,6 +2886,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>35</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -2900,6 +2901,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>35</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -2912,6 +2916,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>35</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -2952,9 +2959,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>35</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -2981,9 +2985,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>35</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -3009,11 +3010,6 @@
       </c>
       <c r="P30">
         <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3023,7 +3019,7 @@
 
 <file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3326,6 +3322,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -3338,6 +3337,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -3350,6 +3352,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -3390,9 +3395,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -3419,9 +3421,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -3447,11 +3446,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5461,7 +5455,7 @@
 
 <file path=xl/worksheets/sheet107.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5875,6 +5869,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -5887,6 +5884,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -5899,6 +5899,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -5939,9 +5942,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -5968,9 +5968,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -5996,11 +5993,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6010,7 +6002,7 @@
 
 <file path=xl/worksheets/sheet108.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6424,6 +6416,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -6436,6 +6431,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -6448,6 +6446,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -6488,9 +6489,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -6517,9 +6515,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -6545,11 +6540,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -7359,7 +7349,7 @@
 
 <file path=xl/worksheets/sheet110.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7773,6 +7763,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -7785,6 +7778,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -7797,6 +7793,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -7837,9 +7836,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -7866,9 +7862,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -7894,11 +7887,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -8308,7 +8296,7 @@
 
 <file path=xl/worksheets/sheet112.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8722,6 +8710,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -8734,6 +8725,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -8746,6 +8740,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -8786,9 +8783,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -8815,9 +8809,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -8843,11 +8834,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -10857,7 +10843,7 @@
 
 <file path=xl/worksheets/sheet118.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11160,6 +11146,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -11172,6 +11161,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -11184,6 +11176,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -11224,9 +11219,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -11253,9 +11245,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -11281,11 +11270,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -11295,7 +11279,7 @@
 
 <file path=xl/worksheets/sheet119.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11598,6 +11582,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -11610,6 +11597,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -11622,6 +11612,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -11662,9 +11655,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -11691,9 +11681,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -11719,11 +11706,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -13655,7 +13637,7 @@
 
 <file path=xl/worksheets/sheet124.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14069,6 +14051,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -14081,6 +14066,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -14093,6 +14081,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -14133,9 +14124,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -14162,9 +14150,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -14190,11 +14175,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -17004,7 +16984,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17307,6 +17287,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -17319,6 +17302,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>20</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -17331,6 +17317,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>20</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -17371,9 +17360,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>20</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -17400,9 +17386,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>20</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -17428,11 +17411,6 @@
       </c>
       <c r="P30">
         <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -17442,7 +17420,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17745,6 +17723,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -17757,6 +17738,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -17769,6 +17753,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -17809,9 +17796,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -17838,9 +17822,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -17866,11 +17847,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -17880,7 +17856,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -18183,6 +18159,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -18195,6 +18174,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -18207,6 +18189,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -18247,9 +18232,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -18276,9 +18258,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -18304,11 +18283,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -20766,7 +20740,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -21069,6 +21043,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -21081,6 +21058,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -21093,6 +21073,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -21133,9 +21116,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -21162,9 +21142,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -21190,11 +21167,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -24804,7 +24776,7 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -25218,6 +25190,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -25230,6 +25205,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -25242,6 +25220,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -25282,9 +25263,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -25311,9 +25289,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -25339,11 +25314,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -25353,7 +25323,7 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -25767,6 +25737,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -25779,6 +25752,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -25791,6 +25767,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -25831,9 +25810,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -25860,9 +25836,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -25888,11 +25861,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -25902,7 +25870,7 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -26316,6 +26284,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -26328,6 +26299,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -26340,6 +26314,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -26380,9 +26357,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -26409,9 +26383,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -26437,11 +26408,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -26851,7 +26817,7 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -27265,6 +27231,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -27277,6 +27246,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -27289,6 +27261,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -27329,9 +27304,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -27358,9 +27330,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -27386,11 +27355,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -29400,7 +29364,7 @@
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -29703,6 +29667,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -29715,6 +29682,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -29727,6 +29697,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -29767,9 +29740,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -29796,9 +29766,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -29824,11 +29791,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -34238,7 +34200,7 @@
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -34541,6 +34503,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -34553,6 +34518,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -34565,6 +34533,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -34605,9 +34576,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -34634,9 +34602,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -34662,11 +34627,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -34676,7 +34636,7 @@
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -34979,6 +34939,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -34991,6 +34954,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -35003,6 +34969,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -35043,9 +35012,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>10</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -35072,9 +35038,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>10</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -35100,11 +35063,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -36314,7 +36272,7 @@
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -36728,6 +36686,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -36740,6 +36701,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -36752,6 +36716,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -36792,9 +36759,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -36821,9 +36785,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -36849,11 +36810,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -36863,7 +36819,7 @@
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -37277,6 +37233,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -37289,6 +37248,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -37301,6 +37263,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -37341,9 +37306,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -37370,9 +37332,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -37398,11 +37357,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -37412,7 +37366,7 @@
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -37826,6 +37780,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -37838,6 +37795,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -37850,6 +37810,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -37890,9 +37853,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -37919,9 +37879,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -37947,11 +37904,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -37961,7 +37913,7 @@
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -38264,6 +38216,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -38276,6 +38231,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -38288,6 +38246,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -38328,9 +38289,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -38357,9 +38315,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -38385,11 +38340,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -38399,7 +38349,7 @@
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -38702,6 +38652,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -38714,6 +38667,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -38726,6 +38682,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -38766,9 +38725,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -38795,9 +38751,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -38823,11 +38776,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -38837,7 +38785,7 @@
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -39140,6 +39088,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -39152,6 +39103,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -39164,6 +39118,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -39204,9 +39161,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -39233,9 +39187,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -39261,11 +39212,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -39275,7 +39221,7 @@
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -39578,6 +39524,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -39590,6 +39539,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -39602,6 +39554,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -39642,9 +39597,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -39671,9 +39623,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -39699,11 +39648,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -39713,7 +39657,7 @@
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -40016,6 +39960,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -40028,6 +39975,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -40040,6 +39990,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -40080,9 +40033,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -40109,9 +40059,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -40137,11 +40084,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -40151,7 +40093,7 @@
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -40565,6 +40507,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -40577,6 +40522,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -40589,6 +40537,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -40629,9 +40580,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -40658,9 +40606,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -40686,11 +40631,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -41100,7 +41040,7 @@
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -41562,6 +41502,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -41574,6 +41517,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -41586,6 +41532,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -41626,9 +41575,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -41655,9 +41601,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -41683,11 +41626,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -42497,7 +42435,7 @@
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -42959,6 +42897,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -42971,6 +42912,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -42983,6 +42927,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -43023,9 +42970,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -43052,9 +42996,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -43080,11 +43021,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -43094,7 +43030,7 @@
 
 <file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -43508,6 +43444,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -43520,6 +43459,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -43532,6 +43474,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -43572,9 +43517,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -43601,9 +43543,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -43629,11 +43568,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -44043,7 +43977,7 @@
 
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -44457,6 +44391,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -44469,6 +44406,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -44481,6 +44421,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -44521,9 +44464,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -44550,9 +44490,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -44578,11 +44515,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -44592,7 +44524,7 @@
 
 <file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -45006,6 +44938,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -45018,6 +44953,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -45030,6 +44968,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -45070,9 +45011,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -45099,9 +45037,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -45127,11 +45062,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -45141,7 +45071,7 @@
 
 <file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -45555,6 +45485,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -45567,6 +45500,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -45579,6 +45515,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -45619,9 +45558,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -45648,9 +45584,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -45676,11 +45609,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -45690,7 +45618,7 @@
 
 <file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -46104,6 +46032,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -46116,6 +46047,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -46128,6 +46062,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -46168,9 +46105,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -46197,9 +46131,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -46225,11 +46156,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -46639,7 +46565,7 @@
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -47053,6 +46979,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -47065,6 +46994,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -47077,6 +47009,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -47117,9 +47052,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -47146,9 +47078,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -47174,11 +47103,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -47188,7 +47112,7 @@
 
 <file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -47491,6 +47415,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -47503,6 +47430,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -47515,6 +47445,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -47555,9 +47488,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -47584,9 +47514,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -47612,11 +47539,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -47626,7 +47548,7 @@
 
 <file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -48040,6 +47962,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -48052,6 +47977,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -48064,6 +47992,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -48104,9 +48035,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -48133,9 +48061,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -48161,11 +48086,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -48175,7 +48095,7 @@
 
 <file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -48478,6 +48398,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -48490,6 +48413,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -48502,6 +48428,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -48542,9 +48471,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -48571,9 +48497,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -48599,11 +48522,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -48613,7 +48531,7 @@
 
 <file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -48916,6 +48834,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -48928,6 +48849,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -48940,6 +48864,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -48980,9 +48907,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -49009,9 +48933,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -49037,11 +48958,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -49051,7 +48967,7 @@
 
 <file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -49354,6 +49270,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -49366,6 +49285,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -49378,6 +49300,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -49418,9 +49343,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -49447,9 +49369,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -49475,11 +49394,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -49489,7 +49403,7 @@
 
 <file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -49792,6 +49706,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -49804,6 +49721,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -49816,6 +49736,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -49856,9 +49779,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -49885,9 +49805,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -49913,11 +49830,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -49927,7 +49839,7 @@
 
 <file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -50230,6 +50142,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -50242,6 +50157,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -50254,6 +50172,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -50294,9 +50215,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -50323,9 +50241,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -50351,11 +50266,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -50365,7 +50275,7 @@
 
 <file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -50668,6 +50578,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -50680,6 +50593,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -50692,6 +50608,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -50732,9 +50651,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -50761,9 +50677,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -50789,11 +50702,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -50803,7 +50711,7 @@
 
 <file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -51217,6 +51125,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -51229,6 +51140,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -51241,6 +51155,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -51281,9 +51198,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -51310,9 +51224,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -51338,11 +51249,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -51752,7 +51658,7 @@
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -52055,6 +51961,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -52067,6 +51976,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -52079,6 +51991,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -52119,9 +52034,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -52148,9 +52060,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -52176,11 +52085,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -52190,7 +52094,7 @@
 
 <file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -52493,6 +52397,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -52505,6 +52412,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -52517,6 +52427,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -52557,9 +52470,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -52586,9 +52496,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -52614,11 +52521,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -52628,7 +52530,7 @@
 
 <file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -52931,6 +52833,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -52943,6 +52848,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -52955,6 +52863,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -52995,9 +52906,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -53024,9 +52932,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -53052,11 +52957,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -53066,7 +52966,7 @@
 
 <file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -53369,6 +53269,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -53381,6 +53284,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>30</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -53393,6 +53299,9 @@
       <c r="P26">
         <v>35</v>
       </c>
+      <c r="Q26">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -53433,9 +53342,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>30</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -53462,9 +53368,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>30</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -53490,11 +53393,6 @@
       </c>
       <c r="P30">
         <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -54800,7 +54698,7 @@
 
 <file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -55214,6 +55112,9 @@
       <c r="D26">
         <v>10</v>
       </c>
+      <c r="E26">
+        <v>35</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -55226,6 +55127,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>35</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -55238,6 +55142,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>35</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -55278,9 +55185,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>35</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -55307,9 +55211,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>35</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -55335,11 +55236,6 @@
       </c>
       <c r="P30">
         <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -55749,7 +55645,7 @@
 
 <file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -56163,6 +56059,9 @@
       <c r="D26">
         <v>30</v>
       </c>
+      <c r="E26">
+        <v>35</v>
+      </c>
       <c r="G26" s="1">
         <v>60</v>
       </c>
@@ -56175,6 +56074,9 @@
       <c r="J26">
         <v>30</v>
       </c>
+      <c r="K26">
+        <v>35</v>
+      </c>
       <c r="M26" s="1">
         <v>40</v>
       </c>
@@ -56187,6 +56089,9 @@
       <c r="P26">
         <v>30</v>
       </c>
+      <c r="Q26">
+        <v>35</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="1">
@@ -56227,9 +56132,6 @@
       </c>
     </row>
     <row r="28" spans="1:17">
-      <c r="E28">
-        <v>35</v>
-      </c>
       <c r="G28" s="1">
         <v>20</v>
       </c>
@@ -56256,9 +56158,6 @@
       </c>
     </row>
     <row r="29" spans="1:17">
-      <c r="K29">
-        <v>35</v>
-      </c>
       <c r="M29" s="1">
         <v>4</v>
       </c>
@@ -56284,11 +56183,6 @@
       </c>
       <c r="P30">
         <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="Q31">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
route 117 and 102 wild pokemon
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="55"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="60"/>
   </bookViews>
   <sheets>
     <sheet name="AbandonedShip_HiddenFloorCorr" sheetId="1" state="visible" r:id="rId2"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="392">
   <si>
     <t xml:space="preserve">map</t>
   </si>
@@ -724,10 +724,16 @@
     <t xml:space="preserve">LOTAD</t>
   </si>
   <si>
-    <t xml:space="preserve">RALTS</t>
+    <t xml:space="preserve">SEEDOT</t>
   </si>
   <si>
-    <t xml:space="preserve">SEEDOT</t>
+    <t xml:space="preserve">CATERPIE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GALARIAN_ZIGZAGOON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RALTS</t>
   </si>
   <si>
     <t xml:space="preserve">MAP_ROUTE103</t>
@@ -874,10 +880,16 @@
     <t xml:space="preserve">gRoute117</t>
   </si>
   <si>
-    <t xml:space="preserve">ILLUMISE</t>
+    <t xml:space="preserve">TRIFOX</t>
   </si>
   <si>
-    <t xml:space="preserve">VOLBEAT</t>
+    <t xml:space="preserve">PUDDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZURILL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILTANK</t>
   </si>
   <si>
     <t xml:space="preserve">MAP_ROUTE118</t>
@@ -1052,9 +1064,6 @@
   </si>
   <si>
     <t xml:space="preserve">HOOTHOOT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MILTANK</t>
   </si>
   <si>
     <t xml:space="preserve">MAP_SAFARI_ZONE_NORTHWEST</t>
@@ -2333,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2350,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,7 +2416,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>25</v>
@@ -2422,7 +2431,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -2442,7 +2451,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>27</v>
@@ -2454,7 +2463,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -2471,7 +2480,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -2483,7 +2492,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -2500,7 +2509,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>27</v>
@@ -2512,7 +2521,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -2529,7 +2538,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
@@ -2541,7 +2550,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -2558,7 +2567,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>27</v>
@@ -2572,7 +2581,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>25</v>
@@ -2586,7 +2595,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>27</v>
@@ -2600,7 +2609,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -2614,7 +2623,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -2628,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -2642,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -2811,7 +2820,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -2825,7 +2834,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -2839,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>25</v>
@@ -2895,7 +2904,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2903,7 +2912,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3346,7 +3355,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3354,7 +3363,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3761,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3769,7 +3778,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4176,7 +4185,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4184,7 +4193,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4591,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4599,7 +4608,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5006,7 +5015,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5014,7 +5023,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5421,7 +5430,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5429,7 +5438,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5983,7 +5992,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5991,7 +6000,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6545,7 +6554,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6553,7 +6562,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7375,7 +7384,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7383,7 +7392,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7484,7 +7493,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -7525,7 +7534,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>25</v>
@@ -7542,7 +7551,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -7554,7 +7563,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>25</v>
@@ -7583,7 +7592,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -7600,7 +7609,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -7628,7 +7637,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -7656,7 +7665,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -7684,7 +7693,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -7937,7 +7946,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7945,7 +7954,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8034,7 +8043,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -8074,7 +8083,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -8114,7 +8123,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -8128,7 +8137,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>26</v>
@@ -8142,7 +8151,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -8170,7 +8179,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>28</v>
@@ -8198,7 +8207,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>30</v>
@@ -8352,7 +8361,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8360,7 +8369,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8461,7 +8470,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -8502,7 +8511,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>25</v>
@@ -8519,7 +8528,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -8531,7 +8540,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>25</v>
@@ -8560,7 +8569,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -8577,7 +8586,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -8605,7 +8614,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -8633,7 +8642,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -8661,7 +8670,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -8914,7 +8923,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8922,7 +8931,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9011,7 +9020,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -9051,7 +9060,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -9091,7 +9100,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -9119,7 +9128,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -9147,7 +9156,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -9175,7 +9184,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -9329,7 +9338,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9337,7 +9346,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9426,7 +9435,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -9466,7 +9475,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -9506,7 +9515,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -9534,7 +9543,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -9562,7 +9571,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -9590,7 +9599,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -9744,7 +9753,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9752,7 +9761,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9901,7 +9910,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -9921,7 +9930,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -9935,7 +9944,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -9949,7 +9958,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -9963,7 +9972,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -9977,7 +9986,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -9991,7 +10000,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10005,7 +10014,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10159,7 +10168,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10167,7 +10176,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10316,7 +10325,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10336,7 +10345,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10350,7 +10359,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10364,7 +10373,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10378,7 +10387,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10392,7 +10401,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10406,7 +10415,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10420,7 +10429,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10574,7 +10583,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10582,7 +10591,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10731,7 +10740,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10751,7 +10760,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10765,7 +10774,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10779,7 +10788,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10793,7 +10802,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10807,7 +10816,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10821,7 +10830,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>39</v>
@@ -10835,7 +10844,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>39</v>
@@ -10989,7 +10998,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10997,7 +11006,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11440,7 +11449,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11448,7 +11457,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11807,7 +11816,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>35</v>
@@ -11821,7 +11830,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -11835,7 +11844,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>5</v>
@@ -12306,7 +12315,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12314,7 +12323,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12383,7 +12392,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12406,7 +12415,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12426,7 +12435,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12446,7 +12455,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12466,7 +12475,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -12658,7 +12667,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12666,7 +12675,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12735,7 +12744,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12758,7 +12767,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12778,7 +12787,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12798,7 +12807,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12818,7 +12827,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -13010,7 +13019,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13018,7 +13027,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13107,7 +13116,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13127,7 +13136,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13215,7 +13224,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38</v>
@@ -13425,7 +13434,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13433,7 +13442,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13534,7 +13543,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13563,7 +13572,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13592,7 +13601,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -13650,7 +13659,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38</v>
@@ -13678,7 +13687,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>42</v>
@@ -13692,7 +13701,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -13706,7 +13715,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -13720,7 +13729,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>42</v>
@@ -13734,7 +13743,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -13888,7 +13897,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13896,7 +13905,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14026,7 +14035,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -14055,7 +14064,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -14155,7 +14164,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -14169,7 +14178,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>42</v>
@@ -14183,7 +14192,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>44</v>
@@ -14197,7 +14206,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>44</v>
@@ -34742,7 +34751,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -37332,7 +37341,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -37435,7 +37444,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>3</v>
@@ -37470,7 +37479,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>3</v>
@@ -37528,7 +37537,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>4</v>
@@ -37557,7 +37566,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>3</v>
@@ -37586,7 +37595,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>4</v>
@@ -37628,7 +37637,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>4</v>
@@ -37642,7 +37651,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>4</v>
@@ -37656,7 +37665,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>4</v>
@@ -37670,7 +37679,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>3</v>
@@ -37923,7 +37932,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37931,7 +37940,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38148,7 +38157,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>3</v>
@@ -38162,7 +38171,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>3</v>
@@ -38176,7 +38185,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>4</v>
@@ -38485,7 +38494,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38493,7 +38502,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39047,7 +39056,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39055,7 +39064,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39498,7 +39507,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39506,7 +39515,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39949,7 +39958,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39957,7 +39966,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40400,7 +40409,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40408,7 +40417,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40851,7 +40860,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40859,7 +40868,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41302,7 +41311,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41310,7 +41319,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41411,7 +41420,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>12</v>
@@ -41440,7 +41449,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>12</v>
@@ -41469,7 +41478,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>13</v>
@@ -41498,7 +41507,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>13</v>
@@ -41527,7 +41536,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>13</v>
@@ -41541,7 +41550,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>13</v>
@@ -41555,7 +41564,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>13</v>
@@ -41597,7 +41606,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>12</v>
@@ -41611,7 +41620,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>13</v>
@@ -42279,7 +42288,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42287,7 +42296,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42514,7 +42523,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>19</v>
@@ -42552,7 +42561,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>21</v>
@@ -42594,7 +42603,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>20</v>
@@ -42608,7 +42617,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>20</v>
@@ -42622,7 +42631,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>22</v>
@@ -42636,7 +42645,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>22</v>
@@ -42889,7 +42898,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42897,7 +42906,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43304,7 +43313,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43312,7 +43321,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43378,7 +43387,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>15</v>
@@ -43401,7 +43410,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>15</v>
@@ -43441,7 +43450,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>14</v>
@@ -43461,7 +43470,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>14</v>
@@ -43495,7 +43504,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>16</v>
@@ -43523,7 +43532,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>16</v>
@@ -43537,7 +43546,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>16</v>
@@ -43551,7 +43560,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>16</v>
@@ -43565,7 +43574,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>16</v>
@@ -43719,7 +43728,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43727,7 +43736,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43793,7 +43802,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>16</v>
@@ -43878,7 +43887,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>17</v>
@@ -43916,7 +43925,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>15</v>
@@ -43992,7 +44001,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>16</v>
@@ -44006,7 +44015,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>16</v>
@@ -44020,7 +44029,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>18</v>
@@ -44034,7 +44043,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>17</v>
@@ -44048,7 +44057,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>15</v>
@@ -44062,7 +44071,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>17</v>
@@ -44076,7 +44085,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>15</v>
@@ -44329,7 +44338,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44337,7 +44346,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44403,7 +44412,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>23</v>
@@ -44467,7 +44476,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -44554,7 +44563,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>25</v>
@@ -44568,7 +44577,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>24</v>
@@ -44582,7 +44591,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>25</v>
@@ -44891,7 +44900,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44899,7 +44908,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45008,7 +45017,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>6</v>
@@ -45048,7 +45057,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>7</v>
@@ -45138,7 +45147,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>7</v>
@@ -45152,7 +45161,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>8</v>
@@ -45306,7 +45315,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45314,7 +45323,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45380,13 +45389,13 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>245</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>20</v>
@@ -45415,13 +45424,13 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>30</v>
@@ -45444,13 +45453,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>180</v>
+        <v>245</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
@@ -45473,13 +45482,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -45502,13 +45511,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>176</v>
+        <v>247</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
@@ -45531,13 +45540,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>215</v>
+        <v>247</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45545,13 +45554,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>243</v>
+        <v>62</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45559,41 +45568,41 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>243</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45601,13 +45610,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45615,13 +45624,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>194</v>
+        <v>248</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45868,7 +45877,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45876,7 +45885,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45977,7 +45986,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>24</v>
@@ -46035,7 +46044,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>26</v>
@@ -46064,7 +46073,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>26</v>
@@ -46093,7 +46102,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -46177,7 +46186,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -46320,7 +46329,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>30</v>
@@ -46334,7 +46343,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>10</v>
@@ -46346,7 +46355,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>20</v>
@@ -46360,7 +46369,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -46374,7 +46383,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>40</v>
@@ -46430,7 +46439,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46438,7 +46447,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46539,7 +46548,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>25</v>
@@ -46597,7 +46606,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>25</v>
@@ -46626,7 +46635,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -46655,7 +46664,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -46669,7 +46678,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>27</v>
@@ -46683,7 +46692,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>24</v>
@@ -46697,7 +46706,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -46711,7 +46720,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>26</v>
@@ -46725,7 +46734,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -46739,7 +46748,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -46841,7 +46850,7 @@
         <v>40</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="O26" s="0" t="n">
         <v>25</v>
@@ -46882,7 +46891,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>30</v>
@@ -46896,7 +46905,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>10</v>
@@ -46908,7 +46917,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>20</v>
@@ -46922,7 +46931,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -46936,7 +46945,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>40</v>
@@ -46992,7 +47001,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47000,7 +47009,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47101,7 +47110,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>25</v>
@@ -47130,7 +47139,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>27</v>
@@ -47159,7 +47168,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>25</v>
@@ -47217,7 +47226,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -47231,7 +47240,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>27</v>
@@ -47259,7 +47268,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -47273,7 +47282,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -47287,7 +47296,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>25</v>
@@ -47301,7 +47310,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -47969,7 +47978,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47977,7 +47986,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48107,7 +48116,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>26</v>
@@ -48165,7 +48174,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>28</v>
@@ -48194,7 +48203,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -48208,7 +48217,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>28</v>
@@ -48222,7 +48231,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>28</v>
@@ -48278,7 +48287,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -48531,7 +48540,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48539,7 +48548,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48982,7 +48991,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48990,7 +48999,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49120,7 +49129,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>26</v>
@@ -49178,7 +49187,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>28</v>
@@ -49207,7 +49216,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -49221,7 +49230,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>28</v>
@@ -49235,7 +49244,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>28</v>
@@ -49291,7 +49300,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -49544,7 +49553,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49552,7 +49561,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49995,7 +50004,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50003,7 +50012,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50446,7 +50455,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50454,7 +50463,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50897,7 +50906,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50905,7 +50914,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51348,7 +51357,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51356,7 +51365,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51799,7 +51808,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51807,7 +51816,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51959,7 +51968,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -52250,7 +52259,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52258,7 +52267,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52324,7 +52333,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>30</v>
@@ -52359,7 +52368,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>35</v>
@@ -52388,7 +52397,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -52417,7 +52426,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -52446,7 +52455,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>20</v>
@@ -52475,7 +52484,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>45</v>
@@ -52489,7 +52498,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>15</v>
@@ -52503,7 +52512,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>50</v>
@@ -52517,7 +52526,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>10</v>
@@ -52531,7 +52540,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>5</v>
@@ -52545,7 +52554,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>10</v>
@@ -52559,7 +52568,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>5</v>
@@ -53227,7 +53236,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53235,7 +53244,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53678,7 +53687,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53686,7 +53695,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54045,7 +54054,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>25</v>
@@ -54129,7 +54138,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54137,7 +54146,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54496,7 +54505,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>25</v>
@@ -54580,7 +54589,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54588,7 +54597,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54947,7 +54956,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>25</v>
@@ -55031,7 +55040,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55039,7 +55048,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55446,7 +55455,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55454,7 +55463,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55520,7 +55529,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>27</v>
@@ -55555,7 +55564,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>27</v>
@@ -55584,7 +55593,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>29</v>
@@ -55613,7 +55622,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>29</v>
@@ -55642,7 +55651,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -55671,7 +55680,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>29</v>
@@ -55685,7 +55694,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>31</v>
@@ -55699,7 +55708,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>29</v>
@@ -55713,7 +55722,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>29</v>
@@ -55727,7 +55736,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -55741,7 +55750,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>31</v>
@@ -55755,7 +55764,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -55909,7 +55918,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55917,7 +55926,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56105,7 +56114,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>34</v>
@@ -56134,7 +56143,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>33</v>
@@ -56148,7 +56157,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>35</v>
@@ -56190,7 +56199,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>37</v>
@@ -56218,7 +56227,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>40</v>
@@ -56372,7 +56381,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56380,7 +56389,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56446,7 +56455,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>27</v>
@@ -56461,7 +56470,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -56481,7 +56490,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>27</v>
@@ -56493,7 +56502,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -56510,7 +56519,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>29</v>
@@ -56522,7 +56531,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -56539,7 +56548,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>29</v>
@@ -56551,7 +56560,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -56568,7 +56577,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -56580,7 +56589,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -56597,7 +56606,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>29</v>
@@ -56611,7 +56620,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>31</v>
@@ -56625,7 +56634,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>29</v>
@@ -56639,7 +56648,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>29</v>
@@ -56653,7 +56662,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -56667,7 +56676,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>31</v>
@@ -56681,7 +56690,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -56850,7 +56859,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -56864,7 +56873,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -56878,7 +56887,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>25</v>
@@ -56934,7 +56943,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56942,7 +56951,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57008,7 +57017,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>25</v>
@@ -57031,7 +57040,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>27</v>
@@ -57051,7 +57060,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -57071,7 +57080,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>27</v>
@@ -57091,7 +57100,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
@@ -57111,7 +57120,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>25</v>
@@ -57125,7 +57134,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>25</v>
@@ -57139,7 +57148,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>27</v>
@@ -57153,7 +57162,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -57167,7 +57176,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -57181,7 +57190,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -57195,7 +57204,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -57349,7 +57358,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57357,7 +57366,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57423,7 +57432,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>33</v>
@@ -57438,7 +57447,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>25</v>
@@ -57487,7 +57496,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>35</v>
@@ -57557,7 +57566,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>35</v>
@@ -57574,7 +57583,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>33</v>
@@ -57588,7 +57597,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>35</v>
@@ -57602,7 +57611,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>34</v>
@@ -57630,7 +57639,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>37</v>
@@ -57658,7 +57667,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>40</v>
@@ -57801,7 +57810,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>25</v>
@@ -57815,7 +57824,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>30</v>
@@ -57827,7 +57836,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -57841,7 +57850,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>30</v>
@@ -57855,7 +57864,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>35</v>

</xml_diff>

<commit_message>
wild pokemon on route 104 and petalburg woods
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="60"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="75"/>
   </bookViews>
   <sheets>
     <sheet name="AbandonedShip_HiddenFloorCorr" sheetId="1" state="visible" r:id="rId2"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="395">
   <si>
     <t xml:space="preserve">map</t>
   </si>
@@ -685,7 +685,7 @@
     <t xml:space="preserve">gPetalburgWoods</t>
   </si>
   <si>
-    <t xml:space="preserve">POOCHYENA</t>
+    <t xml:space="preserve">TREECKO</t>
   </si>
   <si>
     <t xml:space="preserve">WURMPLE</t>
@@ -700,9 +700,6 @@
     <t xml:space="preserve">CASCOON</t>
   </si>
   <si>
-    <t xml:space="preserve">TAILLOW</t>
-  </si>
-  <si>
     <t xml:space="preserve">SLAKOTH</t>
   </si>
   <si>
@@ -710,6 +707,9 @@
   </si>
   <si>
     <t xml:space="preserve">gRoute101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POOCHYENA</t>
   </si>
   <si>
     <t xml:space="preserve">ZIGZAGOON</t>
@@ -749,6 +749,18 @@
   </si>
   <si>
     <t xml:space="preserve">gRoute104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUDKIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEEDLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZURILL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAILLOW</t>
   </si>
   <si>
     <t xml:space="preserve">MAP_ROUTE105</t>
@@ -880,13 +892,10 @@
     <t xml:space="preserve">gRoute117</t>
   </si>
   <si>
-    <t xml:space="preserve">TRIFOX</t>
-  </si>
-  <si>
     <t xml:space="preserve">PUDDI</t>
   </si>
   <si>
-    <t xml:space="preserve">AZURILL</t>
+    <t xml:space="preserve">MEOWSY</t>
   </si>
   <si>
     <t xml:space="preserve">MILTANK</t>
@@ -2342,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,7 +2359,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,7 +2425,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>25</v>
@@ -2431,7 +2440,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -2451,7 +2460,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>27</v>
@@ -2463,7 +2472,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -2480,7 +2489,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -2492,7 +2501,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -2509,7 +2518,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>27</v>
@@ -2521,7 +2530,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -2538,7 +2547,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
@@ -2550,7 +2559,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -2567,7 +2576,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>27</v>
@@ -2581,7 +2590,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>25</v>
@@ -2595,7 +2604,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>27</v>
@@ -2609,7 +2618,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -2623,7 +2632,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -2637,7 +2646,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -2651,7 +2660,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -2820,7 +2829,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -2834,7 +2843,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -2848,7 +2857,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>25</v>
@@ -2904,7 +2913,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,7 +2921,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3355,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3363,7 +3372,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3770,7 +3779,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3778,7 +3787,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4185,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4193,7 +4202,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4600,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4608,7 +4617,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5015,7 +5024,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5023,7 +5032,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5430,7 +5439,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5438,7 +5447,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5992,7 +6001,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6000,7 +6009,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6554,7 +6563,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6562,7 +6571,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7384,7 +7393,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7392,7 +7401,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7493,7 +7502,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -7534,7 +7543,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>25</v>
@@ -7551,7 +7560,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -7563,7 +7572,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>25</v>
@@ -7592,7 +7601,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -7609,7 +7618,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -7637,7 +7646,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -7665,7 +7674,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -7693,7 +7702,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -7946,7 +7955,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7954,7 +7963,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8043,7 +8052,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -8083,7 +8092,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -8123,7 +8132,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -8137,7 +8146,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>26</v>
@@ -8151,7 +8160,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -8179,7 +8188,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>28</v>
@@ -8207,7 +8216,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>30</v>
@@ -8361,7 +8370,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8369,7 +8378,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8470,7 +8479,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -8511,7 +8520,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>25</v>
@@ -8528,7 +8537,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -8540,7 +8549,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>25</v>
@@ -8569,7 +8578,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -8586,7 +8595,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -8614,7 +8623,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -8642,7 +8651,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -8670,7 +8679,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -8923,7 +8932,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8931,7 +8940,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9020,7 +9029,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -9060,7 +9069,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -9100,7 +9109,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -9128,7 +9137,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -9156,7 +9165,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -9184,7 +9193,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -9338,7 +9347,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9346,7 +9355,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9435,7 +9444,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -9475,7 +9484,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -9515,7 +9524,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -9543,7 +9552,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -9571,7 +9580,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -9599,7 +9608,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -9753,7 +9762,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9761,7 +9770,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9910,7 +9919,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -9930,7 +9939,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -9944,7 +9953,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -9958,7 +9967,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -9972,7 +9981,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -9986,7 +9995,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10000,7 +10009,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10014,7 +10023,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10168,7 +10177,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10176,7 +10185,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10325,7 +10334,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10345,7 +10354,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10359,7 +10368,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10373,7 +10382,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10387,7 +10396,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10401,7 +10410,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10415,7 +10424,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10429,7 +10438,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10583,7 +10592,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10591,7 +10600,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10740,7 +10749,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10760,7 +10769,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10774,7 +10783,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10788,7 +10797,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10802,7 +10811,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10816,7 +10825,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10830,7 +10839,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>39</v>
@@ -10844,7 +10853,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>39</v>
@@ -10998,7 +11007,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11006,7 +11015,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11449,7 +11458,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11457,7 +11466,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11816,7 +11825,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>35</v>
@@ -11830,7 +11839,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -11844,7 +11853,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>5</v>
@@ -12315,7 +12324,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12323,7 +12332,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12392,7 +12401,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12415,7 +12424,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12435,7 +12444,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12455,7 +12464,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12475,7 +12484,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -12667,7 +12676,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12675,7 +12684,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12744,7 +12753,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12767,7 +12776,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12787,7 +12796,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12807,7 +12816,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12827,7 +12836,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -13019,7 +13028,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13027,7 +13036,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13116,7 +13125,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13136,7 +13145,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13224,7 +13233,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38</v>
@@ -13434,7 +13443,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13442,7 +13451,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13543,7 +13552,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13572,7 +13581,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13601,7 +13610,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -13659,7 +13668,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38</v>
@@ -13687,7 +13696,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>42</v>
@@ -13701,7 +13710,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -13715,7 +13724,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -13729,7 +13738,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>42</v>
@@ -13743,7 +13752,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -13897,7 +13906,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13905,7 +13914,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14035,7 +14044,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -14064,7 +14073,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -14164,7 +14173,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -14178,7 +14187,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>42</v>
@@ -14192,7 +14201,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>44</v>
@@ -14206,7 +14215,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>44</v>
@@ -36166,7 +36175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>20</v>
       </c>
@@ -36234,7 +36243,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>6</v>
@@ -36330,7 +36339,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>5</v>
@@ -36358,7 +36367,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>6</v>
@@ -36927,7 +36936,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -36938,7 +36947,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -37041,7 +37050,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>2</v>
@@ -37104,7 +37113,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>3</v>
@@ -37125,7 +37134,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>3</v>
@@ -37155,7 +37164,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>3</v>
@@ -37341,8 +37350,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37508,13 +37517,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
@@ -37537,13 +37546,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -37904,7 +37913,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38006,7 +38015,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2</v>
@@ -38041,7 +38050,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>180</v>
+        <v>67</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>3</v>
@@ -38070,7 +38079,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>3</v>
@@ -38099,7 +38108,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>4</v>
@@ -38199,7 +38208,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>67</v>
+        <v>199</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>3</v>
@@ -38227,7 +38236,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>67</v>
+        <v>199</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2</v>
@@ -38466,7 +38475,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38568,13 +38577,13 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>20</v>
@@ -38603,7 +38612,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>4</v>
@@ -38632,7 +38641,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>5</v>
@@ -38661,7 +38670,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>5</v>
@@ -38690,7 +38699,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>4</v>
@@ -38719,7 +38728,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>5</v>
@@ -38733,7 +38742,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>4</v>
@@ -38747,7 +38756,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>5</v>
@@ -38761,7 +38770,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>67</v>
+        <v>203</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>4</v>
@@ -38775,7 +38784,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>67</v>
+        <v>205</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>4</v>
@@ -38789,7 +38798,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>67</v>
+        <v>203</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>3</v>
@@ -38803,7 +38812,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>67</v>
+        <v>205</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>5</v>
@@ -39056,7 +39065,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39064,7 +39073,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39507,7 +39516,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39515,7 +39524,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39958,7 +39967,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39966,7 +39975,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40409,7 +40418,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40417,7 +40426,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40860,7 +40869,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40868,7 +40877,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41311,7 +41320,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41319,7 +41328,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41385,7 +41394,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>12</v>
@@ -41420,7 +41429,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>12</v>
@@ -41449,7 +41458,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>12</v>
@@ -41478,7 +41487,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>13</v>
@@ -41507,7 +41516,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>13</v>
@@ -41536,7 +41545,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>13</v>
@@ -41550,7 +41559,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>13</v>
@@ -41564,7 +41573,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>13</v>
@@ -41606,7 +41615,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>12</v>
@@ -41620,7 +41629,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>13</v>
@@ -42288,7 +42297,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42296,7 +42305,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42523,7 +42532,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>19</v>
@@ -42561,7 +42570,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>21</v>
@@ -42603,7 +42612,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>20</v>
@@ -42617,7 +42626,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>20</v>
@@ -42631,7 +42640,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>22</v>
@@ -42645,7 +42654,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>22</v>
@@ -42898,7 +42907,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42906,7 +42915,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43313,7 +43322,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43321,7 +43330,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43387,7 +43396,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>15</v>
@@ -43410,7 +43419,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>15</v>
@@ -43450,7 +43459,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>14</v>
@@ -43470,7 +43479,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>14</v>
@@ -43504,7 +43513,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>16</v>
@@ -43532,7 +43541,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>16</v>
@@ -43546,7 +43555,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>16</v>
@@ -43560,7 +43569,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>16</v>
@@ -43574,7 +43583,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>16</v>
@@ -43728,7 +43737,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43736,7 +43745,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43802,7 +43811,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>16</v>
@@ -43887,7 +43896,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>17</v>
@@ -43925,7 +43934,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>15</v>
@@ -44001,7 +44010,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>16</v>
@@ -44015,7 +44024,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>16</v>
@@ -44029,7 +44038,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>18</v>
@@ -44043,7 +44052,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>17</v>
@@ -44057,7 +44066,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>15</v>
@@ -44071,7 +44080,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>17</v>
@@ -44085,7 +44094,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>15</v>
@@ -44338,7 +44347,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44346,7 +44355,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44412,7 +44421,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>23</v>
@@ -44447,7 +44456,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>23</v>
@@ -44476,7 +44485,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -44505,7 +44514,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>24</v>
@@ -44534,7 +44543,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
@@ -44563,7 +44572,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>25</v>
@@ -44577,7 +44586,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>24</v>
@@ -44591,7 +44600,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>25</v>
@@ -44900,7 +44909,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44908,7 +44917,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44974,7 +44983,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>6</v>
@@ -45017,7 +45026,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>6</v>
@@ -45057,7 +45066,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>7</v>
@@ -45077,7 +45086,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>6</v>
@@ -45091,7 +45100,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>7</v>
@@ -45105,7 +45114,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>8</v>
@@ -45119,7 +45128,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>7</v>
@@ -45133,7 +45142,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>8</v>
@@ -45147,7 +45156,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>7</v>
@@ -45161,7 +45170,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>8</v>
@@ -45286,7 +45295,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -45315,7 +45324,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45323,7 +45332,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45389,7 +45398,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>4</v>
@@ -45424,7 +45433,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>4</v>
@@ -45453,7 +45462,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>5</v>
@@ -45482,7 +45491,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>5</v>
@@ -45511,7 +45520,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>247</v>
+        <v>204</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>4</v>
@@ -45540,7 +45549,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>247</v>
+        <v>204</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>4</v>
@@ -45582,13 +45591,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>246</v>
+        <v>62</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45596,7 +45605,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>6</v>
@@ -45610,13 +45619,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>248</v>
+        <v>62</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45624,7 +45633,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>7</v>
@@ -45877,7 +45886,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45885,7 +45894,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45986,7 +45995,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>24</v>
@@ -46044,7 +46053,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>26</v>
@@ -46073,7 +46082,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>26</v>
@@ -46102,7 +46111,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -46186,7 +46195,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -46329,7 +46338,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>30</v>
@@ -46343,7 +46352,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>10</v>
@@ -46355,7 +46364,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>20</v>
@@ -46369,7 +46378,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -46383,7 +46392,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>40</v>
@@ -46439,7 +46448,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46447,7 +46456,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46548,7 +46557,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>25</v>
@@ -46606,7 +46615,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>25</v>
@@ -46635,7 +46644,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -46664,7 +46673,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -46678,7 +46687,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>27</v>
@@ -46692,7 +46701,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>24</v>
@@ -46706,7 +46715,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -46720,7 +46729,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>26</v>
@@ -46734,7 +46743,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -46748,7 +46757,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -46850,7 +46859,7 @@
         <v>40</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O26" s="0" t="n">
         <v>25</v>
@@ -46891,7 +46900,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>30</v>
@@ -46905,7 +46914,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>10</v>
@@ -46917,7 +46926,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>20</v>
@@ -46931,7 +46940,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -46945,7 +46954,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>40</v>
@@ -47001,7 +47010,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47009,7 +47018,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47075,7 +47084,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>25</v>
@@ -47110,7 +47119,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>25</v>
@@ -47139,7 +47148,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>27</v>
@@ -47168,7 +47177,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>25</v>
@@ -47226,7 +47235,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -47240,7 +47249,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>27</v>
@@ -47268,7 +47277,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -47282,7 +47291,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -47296,7 +47305,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>25</v>
@@ -47978,7 +47987,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47986,7 +47995,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48052,7 +48061,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>26</v>
@@ -48116,7 +48125,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>26</v>
@@ -48174,7 +48183,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>28</v>
@@ -48203,7 +48212,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -48217,7 +48226,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>28</v>
@@ -48231,7 +48240,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>28</v>
@@ -48287,7 +48296,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -48540,7 +48549,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48548,7 +48557,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48991,7 +49000,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48999,7 +49008,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49065,7 +49074,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>26</v>
@@ -49129,7 +49138,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>26</v>
@@ -49187,7 +49196,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>28</v>
@@ -49216,7 +49225,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -49230,7 +49239,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>28</v>
@@ -49244,7 +49253,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>28</v>
@@ -49300,7 +49309,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -49553,7 +49562,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49561,7 +49570,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50004,7 +50013,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50012,7 +50021,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50455,7 +50464,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50463,7 +50472,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50906,7 +50915,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50914,7 +50923,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51357,7 +51366,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51365,7 +51374,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51808,7 +51817,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51816,7 +51825,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51968,7 +51977,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -52259,7 +52268,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52267,7 +52276,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52333,7 +52342,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>30</v>
@@ -52368,7 +52377,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>35</v>
@@ -52397,7 +52406,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -52426,7 +52435,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -52455,7 +52464,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>20</v>
@@ -52484,7 +52493,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>45</v>
@@ -52498,7 +52507,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>15</v>
@@ -52512,7 +52521,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>50</v>
@@ -52526,7 +52535,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>10</v>
@@ -52540,7 +52549,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>5</v>
@@ -52554,7 +52563,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>10</v>
@@ -52568,7 +52577,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>5</v>
@@ -53236,7 +53245,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53244,7 +53253,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53687,7 +53696,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53695,7 +53704,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54054,7 +54063,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>25</v>
@@ -54138,7 +54147,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54146,7 +54155,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54505,7 +54514,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>25</v>
@@ -54589,7 +54598,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54597,7 +54606,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54956,7 +54965,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>25</v>
@@ -55040,7 +55049,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55048,7 +55057,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55455,7 +55464,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55463,7 +55472,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55529,7 +55538,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>27</v>
@@ -55564,7 +55573,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>27</v>
@@ -55593,7 +55602,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>29</v>
@@ -55622,7 +55631,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>29</v>
@@ -55651,7 +55660,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -55680,7 +55689,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>29</v>
@@ -55694,7 +55703,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>31</v>
@@ -55708,7 +55717,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>29</v>
@@ -55722,7 +55731,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>29</v>
@@ -55736,7 +55745,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -55750,7 +55759,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>31</v>
@@ -55764,7 +55773,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -55918,7 +55927,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55926,7 +55935,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56114,7 +56123,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>34</v>
@@ -56143,7 +56152,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>33</v>
@@ -56157,7 +56166,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>35</v>
@@ -56199,7 +56208,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>37</v>
@@ -56227,7 +56236,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>40</v>
@@ -56381,7 +56390,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56389,7 +56398,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56455,7 +56464,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>27</v>
@@ -56470,7 +56479,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -56490,7 +56499,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>27</v>
@@ -56502,7 +56511,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -56519,7 +56528,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>29</v>
@@ -56531,7 +56540,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -56548,7 +56557,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>29</v>
@@ -56560,7 +56569,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -56577,7 +56586,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -56589,7 +56598,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -56606,7 +56615,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>29</v>
@@ -56620,7 +56629,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>31</v>
@@ -56634,7 +56643,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>29</v>
@@ -56648,7 +56657,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>29</v>
@@ -56662,7 +56671,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -56676,7 +56685,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>31</v>
@@ -56690,7 +56699,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -56859,7 +56868,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -56873,7 +56882,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -56887,7 +56896,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>25</v>
@@ -56943,7 +56952,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56951,7 +56960,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57017,7 +57026,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>25</v>
@@ -57040,7 +57049,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>27</v>
@@ -57060,7 +57069,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -57080,7 +57089,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>27</v>
@@ -57100,7 +57109,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
@@ -57120,7 +57129,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>25</v>
@@ -57134,7 +57143,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>25</v>
@@ -57148,7 +57157,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>27</v>
@@ -57162,7 +57171,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -57176,7 +57185,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -57190,7 +57199,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -57204,7 +57213,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -57358,7 +57367,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57366,7 +57375,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57432,7 +57441,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>33</v>
@@ -57447,7 +57456,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>25</v>
@@ -57496,7 +57505,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>35</v>
@@ -57566,7 +57575,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>35</v>
@@ -57583,7 +57592,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>33</v>
@@ -57597,7 +57606,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>35</v>
@@ -57611,7 +57620,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>34</v>
@@ -57639,7 +57648,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>37</v>
@@ -57667,7 +57676,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>40</v>
@@ -57810,7 +57819,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>25</v>
@@ -57824,7 +57833,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>30</v>
@@ -57836,7 +57845,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -57850,7 +57859,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>30</v>
@@ -57864,7 +57873,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>35</v>

</xml_diff>

<commit_message>
adjust base stats and learnsets (chicks family, poochyena), trainers (routes 102-103-104-alteringcave-117-rusturftunnel-petalburgwoods), alolan marowak thick club, text paragraph fixes
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="396">
   <si>
     <t xml:space="preserve">map</t>
   </si>
@@ -895,7 +895,7 @@
     <t xml:space="preserve">PUDDI</t>
   </si>
   <si>
-    <t xml:space="preserve">MEOWSY</t>
+    <t xml:space="preserve">TORCHIC</t>
   </si>
   <si>
     <t xml:space="preserve">MILTANK</t>
@@ -1040,6 +1040,9 @@
   </si>
   <si>
     <t xml:space="preserve">gRusturfTunnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BONSLY</t>
   </si>
   <si>
     <t xml:space="preserve">MAP_SAFARI_ZONE_NORTH</t>
@@ -2351,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,7 +2362,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,7 +2443,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -2472,7 +2475,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -2489,7 +2492,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -2501,7 +2504,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -2518,7 +2521,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>27</v>
@@ -2530,7 +2533,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -2547,7 +2550,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
@@ -2559,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -2576,7 +2579,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>27</v>
@@ -2604,7 +2607,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>27</v>
@@ -2618,7 +2621,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -2632,7 +2635,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -2646,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -2660,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -2829,7 +2832,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -2843,7 +2846,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -2857,7 +2860,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>25</v>
@@ -2913,7 +2916,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2921,7 +2924,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3364,7 +3367,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,7 +3375,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3779,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3787,7 +3790,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4194,7 +4197,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4202,7 +4205,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4609,7 +4612,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4617,7 +4620,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5024,7 +5027,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5032,7 +5035,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5439,7 +5442,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5447,7 +5450,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6001,7 +6004,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6009,7 +6012,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6563,7 +6566,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6571,7 +6574,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7393,7 +7396,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7401,7 +7404,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7502,7 +7505,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -7543,7 +7546,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>25</v>
@@ -7560,7 +7563,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -7572,7 +7575,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>25</v>
@@ -7601,7 +7604,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -7618,7 +7621,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -7646,7 +7649,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -7674,7 +7677,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -7702,7 +7705,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -7955,7 +7958,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7963,7 +7966,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8052,7 +8055,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -8092,7 +8095,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -8132,7 +8135,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -8146,7 +8149,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>26</v>
@@ -8160,7 +8163,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -8188,7 +8191,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>28</v>
@@ -8216,7 +8219,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>30</v>
@@ -8370,7 +8373,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8378,7 +8381,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8479,7 +8482,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -8520,7 +8523,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>25</v>
@@ -8537,7 +8540,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -8549,7 +8552,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>25</v>
@@ -8578,7 +8581,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -8595,7 +8598,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -8623,7 +8626,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -8651,7 +8654,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -8679,7 +8682,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -8932,7 +8935,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8940,7 +8943,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9029,7 +9032,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -9069,7 +9072,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -9109,7 +9112,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -9137,7 +9140,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -9165,7 +9168,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -9193,7 +9196,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -9347,7 +9350,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9355,7 +9358,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9444,7 +9447,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -9484,7 +9487,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -9524,7 +9527,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -9552,7 +9555,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -9580,7 +9583,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -9608,7 +9611,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -9762,7 +9765,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9770,7 +9773,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9919,7 +9922,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -9939,7 +9942,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -9953,7 +9956,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -9967,7 +9970,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -9981,7 +9984,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -9995,7 +9998,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10009,7 +10012,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10023,7 +10026,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10177,7 +10180,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10185,7 +10188,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10334,7 +10337,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10354,7 +10357,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10368,7 +10371,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10382,7 +10385,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10396,7 +10399,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10410,7 +10413,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10424,7 +10427,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10438,7 +10441,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10592,7 +10595,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10600,7 +10603,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10749,7 +10752,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10769,7 +10772,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10783,7 +10786,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10797,7 +10800,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10811,7 +10814,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10825,7 +10828,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10839,7 +10842,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>39</v>
@@ -10853,7 +10856,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>39</v>
@@ -11007,7 +11010,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11015,7 +11018,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11458,7 +11461,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11466,7 +11469,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11825,7 +11828,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>35</v>
@@ -11839,7 +11842,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -11853,7 +11856,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>5</v>
@@ -12324,7 +12327,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12332,7 +12335,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12401,7 +12404,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12424,7 +12427,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12444,7 +12447,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12464,7 +12467,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12484,7 +12487,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -12676,7 +12679,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12684,7 +12687,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12753,7 +12756,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12776,7 +12779,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12796,7 +12799,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12816,7 +12819,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12836,7 +12839,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -13028,7 +13031,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13036,7 +13039,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13125,7 +13128,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13145,7 +13148,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13233,7 +13236,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38</v>
@@ -13443,7 +13446,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13451,7 +13454,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13552,7 +13555,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13581,7 +13584,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13610,7 +13613,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -13668,7 +13671,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38</v>
@@ -13696,7 +13699,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>42</v>
@@ -13710,7 +13713,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -13724,7 +13727,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -13738,7 +13741,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>42</v>
@@ -13752,7 +13755,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -13906,7 +13909,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13914,7 +13917,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14044,7 +14047,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -14073,7 +14076,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -14173,7 +14176,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -14187,7 +14190,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>42</v>
@@ -14201,7 +14204,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>44</v>
@@ -14215,7 +14218,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>44</v>
@@ -22102,7 +22105,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22207,10 +22210,10 @@
         <v>22</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>7</v>
@@ -22230,10 +22233,10 @@
         <v>23</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>30</v>
@@ -22250,10 +22253,10 @@
         <v>24</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
@@ -22270,10 +22273,10 @@
         <v>24</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -22290,10 +22293,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
@@ -22310,10 +22313,10 @@
         <v>22</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22324,10 +22327,10 @@
         <v>25</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22338,10 +22341,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22352,10 +22355,10 @@
         <v>26</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22366,10 +22369,10 @@
         <v>27</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22380,10 +22383,10 @@
         <v>26</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22394,10 +22397,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36078,7 +36081,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36183,10 +36186,10 @@
         <v>180</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>20</v>
@@ -36206,10 +36209,10 @@
         <v>181</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>30</v>
@@ -36226,10 +36229,10 @@
         <v>182</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
@@ -36246,10 +36249,10 @@
         <v>182</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -36266,10 +36269,10 @@
         <v>183</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
@@ -36286,10 +36289,10 @@
         <v>184</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36314,10 +36317,10 @@
         <v>182</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36328,10 +36331,10 @@
         <v>185</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36342,10 +36345,10 @@
         <v>185</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36356,10 +36359,10 @@
         <v>185</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36370,10 +36373,10 @@
         <v>185</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37351,7 +37354,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37456,10 +37459,10 @@
         <v>192</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>20</v>
@@ -37491,10 +37494,10 @@
         <v>193</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>30</v>
@@ -37578,10 +37581,10 @@
         <v>194</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
@@ -37607,10 +37610,10 @@
         <v>194</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37621,10 +37624,10 @@
         <v>189</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37635,10 +37638,10 @@
         <v>189</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37649,10 +37652,10 @@
         <v>195</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37663,10 +37666,10 @@
         <v>196</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37677,10 +37680,10 @@
         <v>195</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37691,10 +37694,10 @@
         <v>196</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38475,7 +38478,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38580,10 +38583,10 @@
         <v>202</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>20</v>
@@ -38615,10 +38618,10 @@
         <v>203</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>30</v>
@@ -38673,10 +38676,10 @@
         <v>204</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -38702,10 +38705,10 @@
         <v>205</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
@@ -38745,10 +38748,10 @@
         <v>205</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38759,10 +38762,10 @@
         <v>205</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38773,10 +38776,10 @@
         <v>203</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38787,10 +38790,10 @@
         <v>205</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38801,10 +38804,10 @@
         <v>203</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38815,10 +38818,10 @@
         <v>205</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45401,10 +45404,10 @@
         <v>249</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>20</v>
@@ -45433,13 +45436,13 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>250</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>30</v>
@@ -45465,10 +45468,10 @@
         <v>249</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
@@ -45491,13 +45494,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>250</v>
+        <v>33</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -45520,13 +45523,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>204</v>
+        <v>250</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
@@ -45549,13 +45552,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>204</v>
+        <v>250</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45566,10 +45569,10 @@
         <v>62</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45580,10 +45583,10 @@
         <v>62</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45594,10 +45597,10 @@
         <v>62</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45608,10 +45611,10 @@
         <v>251</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45622,10 +45625,10 @@
         <v>62</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45636,10 +45639,10 @@
         <v>251</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55021,7 +55024,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -55126,10 +55129,10 @@
         <v>63</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>10</v>
@@ -55149,10 +55152,10 @@
         <v>63</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>30</v>
@@ -55169,10 +55172,10 @@
         <v>63</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
@@ -55189,10 +55192,10 @@
         <v>63</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -55209,10 +55212,10 @@
         <v>63</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
@@ -55229,10 +55232,10 @@
         <v>63</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55240,13 +55243,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>63</v>
+        <v>299</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55254,13 +55257,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>63</v>
+        <v>299</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55268,13 +55271,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>63</v>
+        <v>299</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55282,13 +55285,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>63</v>
+        <v>299</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55296,13 +55299,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>63</v>
+        <v>299</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55310,13 +55313,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>63</v>
+        <v>299</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55464,7 +55467,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55472,7 +55475,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55538,7 +55541,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>27</v>
@@ -55602,7 +55605,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>29</v>
@@ -55660,7 +55663,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -55717,7 +55720,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>29</v>
@@ -55731,7 +55734,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>29</v>
@@ -55745,7 +55748,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -55759,7 +55762,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>31</v>
@@ -55773,7 +55776,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -55927,7 +55930,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55935,7 +55938,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56123,7 +56126,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>34</v>
@@ -56152,7 +56155,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>33</v>
@@ -56166,7 +56169,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>35</v>
@@ -56390,7 +56393,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56398,7 +56401,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56464,7 +56467,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>27</v>
@@ -56479,7 +56482,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -56511,7 +56514,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -56528,7 +56531,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>29</v>
@@ -56540,7 +56543,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -56569,7 +56572,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -56586,7 +56589,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -56598,7 +56601,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -56643,7 +56646,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>29</v>
@@ -56657,7 +56660,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>29</v>
@@ -56671,7 +56674,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -56685,7 +56688,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>31</v>
@@ -56699,7 +56702,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -56868,7 +56871,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -56882,7 +56885,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -56896,7 +56899,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>25</v>
@@ -56952,7 +56955,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56960,7 +56963,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57069,7 +57072,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -57089,7 +57092,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>27</v>
@@ -57109,7 +57112,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
@@ -57129,7 +57132,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>25</v>
@@ -57157,7 +57160,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>27</v>
@@ -57171,7 +57174,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -57185,7 +57188,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -57199,7 +57202,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -57213,7 +57216,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -57367,7 +57370,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57375,7 +57378,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57441,7 +57444,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>33</v>
@@ -57456,7 +57459,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>25</v>
@@ -57505,7 +57508,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>35</v>
@@ -57575,7 +57578,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>35</v>
@@ -57592,7 +57595,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>33</v>
@@ -57606,7 +57609,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>35</v>
@@ -57620,7 +57623,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>34</v>
@@ -57648,7 +57651,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>37</v>
@@ -57676,7 +57679,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>40</v>
@@ -57819,7 +57822,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>25</v>
@@ -57833,7 +57836,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>30</v>
@@ -57845,7 +57848,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -57859,7 +57862,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>30</v>
@@ -57873,7 +57876,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>35</v>

</xml_diff>

<commit_message>
route 116 wild pokemon
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="75"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="74"/>
   </bookViews>
   <sheets>
     <sheet name="AbandonedShip_HiddenFloorCorr" sheetId="1" state="visible" r:id="rId2"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="399">
   <si>
     <t xml:space="preserve">map</t>
   </si>
@@ -880,10 +880,19 @@
     <t xml:space="preserve">gRoute116</t>
   </si>
   <si>
+    <t xml:space="preserve">CYNDAQUIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEOWSY</t>
+  </si>
+  <si>
     <t xml:space="preserve">NINCADA</t>
   </si>
   <si>
     <t xml:space="preserve">SKITTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEVEE</t>
   </si>
   <si>
     <t xml:space="preserve">MAP_ROUTE117</t>
@@ -2354,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,7 +2371,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,7 +2452,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -2475,7 +2484,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -2492,7 +2501,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -2504,7 +2513,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -2521,7 +2530,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>27</v>
@@ -2533,7 +2542,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -2550,7 +2559,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
@@ -2562,7 +2571,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -2579,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>27</v>
@@ -2593,7 +2602,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>25</v>
@@ -2607,7 +2616,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>27</v>
@@ -2621,7 +2630,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -2635,7 +2644,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -2649,7 +2658,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -2663,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -2832,7 +2841,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -2846,7 +2855,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -2860,7 +2869,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>25</v>
@@ -2916,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,7 +2933,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3367,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3375,7 +3384,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3782,7 +3791,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3790,7 +3799,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4197,7 +4206,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4205,7 +4214,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4612,7 +4621,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4620,7 +4629,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5027,7 +5036,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5035,7 +5044,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5442,7 +5451,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5450,7 +5459,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6004,7 +6013,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6012,7 +6021,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6566,7 +6575,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6574,7 +6583,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7396,7 +7405,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7404,7 +7413,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7505,7 +7514,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -7546,7 +7555,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>25</v>
@@ -7563,7 +7572,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -7575,7 +7584,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>25</v>
@@ -7604,7 +7613,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -7621,7 +7630,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -7649,7 +7658,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -7677,7 +7686,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -7705,7 +7714,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -7958,7 +7967,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7966,7 +7975,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8055,7 +8064,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -8095,7 +8104,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -8135,7 +8144,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -8149,7 +8158,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>26</v>
@@ -8163,7 +8172,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -8191,7 +8200,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>28</v>
@@ -8219,7 +8228,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>30</v>
@@ -8373,7 +8382,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8381,7 +8390,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8482,7 +8491,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -8523,7 +8532,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>25</v>
@@ -8540,7 +8549,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -8552,7 +8561,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>25</v>
@@ -8581,7 +8590,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -8598,7 +8607,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -8626,7 +8635,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -8654,7 +8663,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -8682,7 +8691,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -8935,7 +8944,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8943,7 +8952,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9032,7 +9041,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -9072,7 +9081,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -9112,7 +9121,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -9140,7 +9149,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -9168,7 +9177,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -9196,7 +9205,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -9350,7 +9359,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9358,7 +9367,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9447,7 +9456,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>26</v>
@@ -9487,7 +9496,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -9527,7 +9536,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>30</v>
@@ -9555,7 +9564,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>32</v>
@@ -9583,7 +9592,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>32</v>
@@ -9611,7 +9620,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>32</v>
@@ -9765,7 +9774,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9773,7 +9782,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9922,7 +9931,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -9942,7 +9951,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -9956,7 +9965,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -9970,7 +9979,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -9984,7 +9993,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -9998,7 +10007,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10012,7 +10021,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10026,7 +10035,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10180,7 +10189,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10188,7 +10197,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10337,7 +10346,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10357,7 +10366,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10371,7 +10380,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10385,7 +10394,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10399,7 +10408,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10413,7 +10422,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10427,7 +10436,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10441,7 +10450,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10595,7 +10604,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10603,7 +10612,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10752,7 +10761,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10772,7 +10781,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10786,7 +10795,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10800,7 +10809,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10814,7 +10823,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10828,7 +10837,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10842,7 +10851,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>39</v>
@@ -10856,7 +10865,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>39</v>
@@ -11010,7 +11019,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11018,7 +11027,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11461,7 +11470,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11469,7 +11478,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11828,7 +11837,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>35</v>
@@ -11842,7 +11851,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -11856,7 +11865,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>5</v>
@@ -12327,7 +12336,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12335,7 +12344,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12404,7 +12413,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12427,7 +12436,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12447,7 +12456,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12467,7 +12476,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12487,7 +12496,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -12679,7 +12688,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12687,7 +12696,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12756,7 +12765,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12779,7 +12788,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12799,7 +12808,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12819,7 +12828,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12839,7 +12848,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -13031,7 +13040,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13039,7 +13048,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13128,7 +13137,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13148,7 +13157,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13236,7 +13245,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38</v>
@@ -13446,7 +13455,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13454,7 +13463,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13555,7 +13564,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13584,7 +13593,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13613,7 +13622,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -13671,7 +13680,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38</v>
@@ -13699,7 +13708,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>42</v>
@@ -13713,7 +13722,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -13727,7 +13736,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -13741,7 +13750,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>42</v>
@@ -13755,7 +13764,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -13909,7 +13918,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13917,7 +13926,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14047,7 +14056,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -14076,7 +14085,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -14176,7 +14185,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -14190,7 +14199,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>42</v>
@@ -14204,7 +14213,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>44</v>
@@ -14218,7 +14227,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>44</v>
@@ -44883,8 +44892,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -44986,13 +44995,13 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>188</v>
+        <v>245</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>20</v>
@@ -45009,13 +45018,13 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>63</v>
+        <v>246</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>30</v>
@@ -45029,13 +45038,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
@@ -45052,10 +45061,10 @@
         <v>85</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -45069,13 +45078,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
@@ -45089,13 +45098,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45103,13 +45112,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45117,13 +45126,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45131,13 +45140,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>188</v>
+        <v>249</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45145,13 +45154,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>188</v>
+        <v>249</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45159,13 +45168,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45173,13 +45182,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45298,8 +45307,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -45327,7 +45336,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45335,7 +45344,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45401,7 +45410,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>9</v>
@@ -45465,7 +45474,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>10</v>
@@ -45523,7 +45532,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>10</v>
@@ -45552,7 +45561,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>10</v>
@@ -45608,7 +45617,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>10</v>
@@ -45636,7 +45645,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>10</v>
@@ -45889,7 +45898,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45897,7 +45906,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46085,7 +46094,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>26</v>
@@ -46114,7 +46123,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>26</v>
@@ -46198,7 +46207,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -46341,7 +46350,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>30</v>
@@ -46355,7 +46364,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>10</v>
@@ -46367,7 +46376,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>20</v>
@@ -46381,7 +46390,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -46395,7 +46404,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>40</v>
@@ -46451,7 +46460,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46459,7 +46468,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46560,7 +46569,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>25</v>
@@ -46647,7 +46656,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -46718,7 +46727,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -46732,7 +46741,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>26</v>
@@ -46746,7 +46755,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -46760,7 +46769,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -46862,7 +46871,7 @@
         <v>40</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O26" s="0" t="n">
         <v>25</v>
@@ -46903,7 +46912,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>30</v>
@@ -46917,7 +46926,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>10</v>
@@ -46929,7 +46938,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>20</v>
@@ -46943,7 +46952,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -46957,7 +46966,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>40</v>
@@ -47013,7 +47022,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47021,7 +47030,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47122,7 +47131,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>25</v>
@@ -47151,7 +47160,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>27</v>
@@ -47280,7 +47289,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -47294,7 +47303,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -47308,7 +47317,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>25</v>
@@ -47990,7 +47999,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47998,7 +48007,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48128,7 +48137,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>26</v>
@@ -48186,7 +48195,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>28</v>
@@ -48243,7 +48252,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>28</v>
@@ -48299,7 +48308,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -48552,7 +48561,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48560,7 +48569,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49003,7 +49012,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49011,7 +49020,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49141,7 +49150,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>26</v>
@@ -49199,7 +49208,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>28</v>
@@ -49256,7 +49265,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>28</v>
@@ -49312,7 +49321,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>25</v>
@@ -49565,7 +49574,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49573,7 +49582,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50016,7 +50025,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50024,7 +50033,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50467,7 +50476,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50475,7 +50484,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50918,7 +50927,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50926,7 +50935,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51369,7 +51378,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51377,7 +51386,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51820,7 +51829,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51828,7 +51837,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51980,7 +51989,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -52271,7 +52280,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52279,7 +52288,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52345,7 +52354,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>30</v>
@@ -52380,7 +52389,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>35</v>
@@ -52409,7 +52418,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -52438,7 +52447,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -52467,7 +52476,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>20</v>
@@ -52496,7 +52505,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>45</v>
@@ -52510,7 +52519,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>15</v>
@@ -52524,7 +52533,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>50</v>
@@ -52538,7 +52547,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>10</v>
@@ -52552,7 +52561,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>5</v>
@@ -52566,7 +52575,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>10</v>
@@ -52580,7 +52589,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>5</v>
@@ -53248,7 +53257,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53256,7 +53265,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53699,7 +53708,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53707,7 +53716,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54066,7 +54075,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>25</v>
@@ -54150,7 +54159,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54158,7 +54167,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54517,7 +54526,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>25</v>
@@ -54601,7 +54610,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54609,7 +54618,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54968,7 +54977,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>25</v>
@@ -55052,7 +55061,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55060,7 +55069,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55243,7 +55252,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>9</v>
@@ -55257,7 +55266,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>9</v>
@@ -55271,7 +55280,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>10</v>
@@ -55285,7 +55294,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>10</v>
@@ -55299,7 +55308,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>10</v>
@@ -55313,7 +55322,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>10</v>
@@ -55467,7 +55476,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55475,7 +55484,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55541,7 +55550,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>27</v>
@@ -55605,7 +55614,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>29</v>
@@ -55663,7 +55672,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -55692,7 +55701,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>29</v>
@@ -55706,7 +55715,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>31</v>
@@ -55720,7 +55729,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>29</v>
@@ -55734,7 +55743,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>29</v>
@@ -55748,7 +55757,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -55762,7 +55771,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>31</v>
@@ -55776,7 +55785,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -55930,7 +55939,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55938,7 +55947,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56126,7 +56135,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>34</v>
@@ -56155,7 +56164,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>33</v>
@@ -56169,7 +56178,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>35</v>
@@ -56211,7 +56220,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>37</v>
@@ -56239,7 +56248,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>40</v>
@@ -56393,7 +56402,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56401,7 +56410,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56467,7 +56476,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>27</v>
@@ -56482,7 +56491,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -56514,7 +56523,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -56531,7 +56540,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>29</v>
@@ -56543,7 +56552,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -56572,7 +56581,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -56589,7 +56598,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>27</v>
@@ -56601,7 +56610,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>25</v>
@@ -56618,7 +56627,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>29</v>
@@ -56632,7 +56641,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>31</v>
@@ -56646,7 +56655,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>29</v>
@@ -56660,7 +56669,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>29</v>
@@ -56674,7 +56683,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -56688,7 +56697,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>31</v>
@@ -56702,7 +56711,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -56871,7 +56880,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -56885,7 +56894,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -56899,7 +56908,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>25</v>
@@ -56955,7 +56964,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -56963,7 +56972,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57072,7 +57081,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>25</v>
@@ -57092,7 +57101,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>27</v>
@@ -57112,7 +57121,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>25</v>
@@ -57132,7 +57141,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>25</v>
@@ -57146,7 +57155,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>25</v>
@@ -57160,7 +57169,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>27</v>
@@ -57174,7 +57183,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>25</v>
@@ -57188,7 +57197,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>27</v>
@@ -57202,7 +57211,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>27</v>
@@ -57216,7 +57225,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>29</v>
@@ -57370,7 +57379,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57378,7 +57387,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57444,7 +57453,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>33</v>
@@ -57459,7 +57468,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>25</v>
@@ -57508,7 +57517,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>35</v>
@@ -57578,7 +57587,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>35</v>
@@ -57595,7 +57604,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>33</v>
@@ -57609,7 +57618,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>35</v>
@@ -57623,7 +57632,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>34</v>
@@ -57651,7 +57660,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>37</v>
@@ -57679,7 +57688,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>40</v>
@@ -57822,7 +57831,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>25</v>
@@ -57836,7 +57845,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>30</v>
@@ -57848,7 +57857,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>30</v>
@@ -57862,7 +57871,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>30</v>
@@ -57876,7 +57885,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>35</v>

</xml_diff>

<commit_message>
try to figure out where the missing definition for silent forest map scripts goes
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="74"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="113"/>
   </bookViews>
   <sheets>
     <sheet name="AbandonedShip_HiddenFloorCorr" sheetId="1" state="visible" r:id="rId2"/>
@@ -121,7 +121,7 @@
     <sheet name="ShoalCave_LowTideIceRoom" sheetId="111" state="visible" r:id="rId112"/>
     <sheet name="ShoalCave_LowTideInnerRoom" sheetId="112" state="visible" r:id="rId113"/>
     <sheet name="ShoalCave_LowTideLowerRoom" sheetId="113" state="visible" r:id="rId114"/>
-    <sheet name="ShoalCave_LowTideStairsRoom" sheetId="114" state="visible" r:id="rId115"/>
+    <sheet name="SilentForest" sheetId="114" state="visible" r:id="rId115"/>
     <sheet name="SkyPillar_1F" sheetId="115" state="visible" r:id="rId116"/>
     <sheet name="SkyPillar_3F" sheetId="116" state="visible" r:id="rId117"/>
     <sheet name="SkyPillar_5F" sheetId="117" state="visible" r:id="rId118"/>
@@ -1246,10 +1246,10 @@
     <t xml:space="preserve">gShoalCave_LowTideLowerRoom</t>
   </si>
   <si>
-    <t xml:space="preserve">MAP_SHOAL_CAVE_LOW_TIDE_STAIRS_ROOM</t>
+    <t xml:space="preserve">MAP_SILENT_FOREST</t>
   </si>
   <si>
-    <t xml:space="preserve">gShoalCave_LowTideStairsRoom</t>
+    <t xml:space="preserve">gSilentForest</t>
   </si>
   <si>
     <t xml:space="preserve">MAP_SKY_PILLAR_1F</t>
@@ -9330,7 +9330,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -44892,7 +44892,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
silent forest scripts and wild pokemon, pikachu evolution method
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6935" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6937" uniqueCount="405">
   <si>
     <t xml:space="preserve">map</t>
   </si>
@@ -1252,6 +1252,24 @@
     <t xml:space="preserve">gSilentForest</t>
   </si>
   <si>
+    <t xml:space="preserve">BULBASAUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIDGEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICHU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLOWPOKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEEBAS</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAP_SKY_PILLAR_1F</t>
   </si>
   <si>
@@ -9331,7 +9349,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9433,16 +9451,16 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>369</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>60</v>
@@ -9456,13 +9474,13 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>359</v>
+        <v>332</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>30</v>
@@ -9476,13 +9494,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>370</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>5</v>
@@ -9496,13 +9514,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>4</v>
@@ -9516,13 +9534,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>371</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>1</v>
@@ -9536,13 +9554,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9550,13 +9568,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>22</v>
+        <v>370</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9564,13 +9582,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9578,13 +9596,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>372</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9592,13 +9610,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9606,13 +9624,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>372</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9620,13 +9638,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9691,6 +9709,18 @@
       <c r="A26" s="1" t="n">
         <v>70</v>
       </c>
+      <c r="B26" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="G26" s="1" t="n">
         <v>60</v>
       </c>
@@ -9701,6 +9731,15 @@
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>30</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>15</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>20</v>
@@ -9774,7 +9813,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9782,7 +9821,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9931,7 +9970,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -9951,7 +9990,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -9965,7 +10004,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -9979,7 +10018,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -9993,7 +10032,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10007,7 +10046,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10021,7 +10060,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10035,7 +10074,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10189,7 +10228,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10197,7 +10236,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10346,7 +10385,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10366,7 +10405,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10380,7 +10419,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10394,7 +10433,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10408,7 +10447,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10422,7 +10461,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10436,7 +10475,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10450,7 +10489,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10604,7 +10643,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10612,7 +10651,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10761,7 +10800,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10781,7 +10820,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10795,7 +10834,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10809,7 +10848,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10823,7 +10862,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10837,7 +10876,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10851,7 +10890,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>39</v>
@@ -10865,7 +10904,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>39</v>
@@ -11019,7 +11058,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11027,7 +11066,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11470,7 +11509,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11478,7 +11517,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11837,7 +11876,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>35</v>
@@ -11851,7 +11890,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -11865,7 +11904,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>5</v>
@@ -12336,7 +12375,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12344,7 +12383,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12413,7 +12452,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12436,7 +12475,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12456,7 +12495,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12476,7 +12515,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12496,7 +12535,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -12688,7 +12727,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12696,7 +12735,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12765,7 +12804,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12788,7 +12827,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12808,7 +12847,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12828,7 +12867,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12848,7 +12887,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -13040,7 +13079,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13048,7 +13087,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13137,7 +13176,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13157,7 +13196,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13245,7 +13284,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38</v>
@@ -13455,7 +13494,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13463,7 +13502,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13564,7 +13603,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13593,7 +13632,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13622,7 +13661,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -13680,7 +13719,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38</v>
@@ -13708,7 +13747,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>42</v>
@@ -13722,7 +13761,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -13736,7 +13775,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -13750,7 +13789,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>42</v>
@@ -13764,7 +13803,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -13918,7 +13957,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13926,7 +13965,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14056,7 +14095,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -14085,7 +14124,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -14185,7 +14224,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -14199,7 +14238,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>42</v>
@@ -14213,7 +14252,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>44</v>
@@ -14227,7 +14266,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>44</v>

</xml_diff>

<commit_message>
add good and super rood encounters to silent forest
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6937" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6945" uniqueCount="407">
   <si>
     <t xml:space="preserve">map</t>
   </si>
@@ -1270,6 +1270,12 @@
     <t xml:space="preserve">FEEBAS</t>
   </si>
   <si>
+    <t xml:space="preserve">SLOWBRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLOWKING</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAP_SKY_PILLAR_1F</t>
   </si>
   <si>
@@ -9348,8 +9354,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O30" activeCellId="0" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9724,9 +9730,27 @@
       <c r="G26" s="1" t="n">
         <v>60</v>
       </c>
+      <c r="H26" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>35</v>
+      </c>
       <c r="M26" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="N26" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -9744,26 +9768,80 @@
       <c r="G27" s="1" t="n">
         <v>20</v>
       </c>
+      <c r="H27" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>35</v>
+      </c>
       <c r="M27" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="N27" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G28" s="1" t="n">
         <v>20</v>
       </c>
+      <c r="H28" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>35</v>
+      </c>
       <c r="M28" s="1" t="n">
         <v>15</v>
       </c>
+      <c r="N28" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M29" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="N29" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="P29" s="0" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M30" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="P30" s="0" t="n">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -9813,7 +9891,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9821,7 +9899,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9970,7 +10048,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -9990,7 +10068,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10004,7 +10082,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10018,7 +10096,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10032,7 +10110,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10046,7 +10124,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10060,7 +10138,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10074,7 +10152,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10228,7 +10306,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10236,7 +10314,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10385,7 +10463,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10405,7 +10483,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10419,7 +10497,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10433,7 +10511,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10447,7 +10525,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10461,7 +10539,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10475,7 +10553,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10489,7 +10567,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10643,7 +10721,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10651,7 +10729,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10800,7 +10878,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10820,7 +10898,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10834,7 +10912,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10848,7 +10926,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10862,7 +10940,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10876,7 +10954,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10890,7 +10968,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>39</v>
@@ -10904,7 +10982,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>39</v>
@@ -11058,7 +11136,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11066,7 +11144,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11509,7 +11587,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11517,7 +11595,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11876,7 +11954,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>35</v>
@@ -11890,7 +11968,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -11904,7 +11982,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>5</v>
@@ -12375,7 +12453,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12383,7 +12461,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12452,7 +12530,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12475,7 +12553,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12495,7 +12573,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12515,7 +12593,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12535,7 +12613,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -12727,7 +12805,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12735,7 +12813,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12804,7 +12882,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12827,7 +12905,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12847,7 +12925,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12867,7 +12945,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12887,7 +12965,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -13079,7 +13157,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13087,7 +13165,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13176,7 +13254,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13196,7 +13274,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13284,7 +13362,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38</v>
@@ -13494,7 +13572,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13502,7 +13580,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13603,7 +13681,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13632,7 +13710,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13661,7 +13739,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -13719,7 +13797,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38</v>
@@ -13747,7 +13825,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>42</v>
@@ -13761,7 +13839,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -13775,7 +13853,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -13789,7 +13867,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>42</v>
@@ -13803,7 +13881,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -13957,7 +14035,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13965,7 +14043,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14095,7 +14173,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -14124,7 +14202,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -14224,7 +14302,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -14238,7 +14316,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>42</v>
@@ -14252,7 +14330,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>44</v>
@@ -14266,7 +14344,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>44</v>

</xml_diff>

<commit_message>
tweak postdoc tutor, silent forest wild pokemon
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6945" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6945" uniqueCount="404">
   <si>
     <t xml:space="preserve">map</t>
   </si>
@@ -1255,6 +1255,9 @@
     <t xml:space="preserve">BULBASAUR</t>
   </si>
   <si>
+    <t xml:space="preserve">GOLPPY</t>
+  </si>
+  <si>
     <t xml:space="preserve">SLOWPOKE</t>
   </si>
   <si>
@@ -9343,7 +9346,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9719,7 +9722,7 @@
         <v>60</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>20</v>
@@ -9731,7 +9734,7 @@
         <v>40</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="O26" s="0" t="n">
         <v>40</v>
@@ -9757,7 +9760,7 @@
         <v>20</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>20</v>
@@ -9769,7 +9772,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>40</v>
@@ -9783,7 +9786,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>20</v>
@@ -9795,7 +9798,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>40</v>
@@ -9809,7 +9812,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>40</v>
@@ -9823,7 +9826,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>40</v>
@@ -9879,7 +9882,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9887,7 +9890,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10036,7 +10039,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10056,7 +10059,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10070,7 +10073,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10084,7 +10087,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10098,7 +10101,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10112,7 +10115,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10126,7 +10129,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10140,7 +10143,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10294,7 +10297,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10302,7 +10305,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10451,7 +10454,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10471,7 +10474,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10485,7 +10488,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10499,7 +10502,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10513,7 +10516,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10527,7 +10530,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10541,7 +10544,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10555,7 +10558,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10709,7 +10712,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10717,7 +10720,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10866,7 +10869,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10886,7 +10889,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10900,7 +10903,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10914,7 +10917,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10928,7 +10931,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10942,7 +10945,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10956,7 +10959,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>39</v>
@@ -10970,7 +10973,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>39</v>
@@ -11124,7 +11127,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11132,7 +11135,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11575,7 +11578,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11583,7 +11586,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11942,7 +11945,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>35</v>
@@ -11956,7 +11959,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -11970,7 +11973,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>5</v>
@@ -12441,7 +12444,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12449,7 +12452,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12518,7 +12521,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12541,7 +12544,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12561,7 +12564,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12581,7 +12584,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12601,7 +12604,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -12793,7 +12796,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12801,7 +12804,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12870,7 +12873,7 @@
         <v>60</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>20</v>
@@ -12893,7 +12896,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -12913,7 +12916,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>30</v>
@@ -12933,7 +12936,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -12953,7 +12956,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -13145,7 +13148,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13153,7 +13156,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13242,7 +13245,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13262,7 +13265,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13350,7 +13353,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38</v>
@@ -13560,7 +13563,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13568,7 +13571,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13669,7 +13672,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13698,7 +13701,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13727,7 +13730,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -13785,7 +13788,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38</v>
@@ -13813,7 +13816,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>42</v>
@@ -13827,7 +13830,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -13841,7 +13844,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -13855,7 +13858,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>42</v>
@@ -13869,7 +13872,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -14023,7 +14026,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14031,7 +14034,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14161,7 +14164,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -14190,7 +14193,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -14290,7 +14293,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -14304,7 +14307,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>42</v>
@@ -14318,7 +14321,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>44</v>
@@ -14332,7 +14335,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>44</v>

</xml_diff>

<commit_message>
fix brine beach map names
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="415">
   <si>
     <t xml:space="preserve">map</t>
   </si>
@@ -287,10 +287,10 @@
     <t xml:space="preserve">gArtisanCave_B1F</t>
   </si>
   <si>
-    <t xml:space="preserve">MAP_SILENT_FOREST</t>
+    <t xml:space="preserve">MAP_BRINE_BEACH</t>
   </si>
   <si>
-    <t xml:space="preserve">gSilentForest</t>
+    <t xml:space="preserve">gBrineBeach</t>
   </si>
   <si>
     <t xml:space="preserve">KRABBY</t>
@@ -1277,6 +1277,12 @@
     <t xml:space="preserve">gShoalCave_LowTideLowerRoom</t>
   </si>
   <si>
+    <t xml:space="preserve">MAP_SILENT_FOREST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gSilentForest</t>
+  </si>
+  <si>
     <t xml:space="preserve">PIDGEY</t>
   </si>
   <si>
@@ -9964,7 +9970,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>47</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9972,7 +9978,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>48</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10061,7 +10067,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>13</v>
@@ -10101,7 +10107,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>14</v>
@@ -10121,7 +10127,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>15</v>
@@ -10141,7 +10147,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>15</v>
@@ -10155,7 +10161,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>15</v>
@@ -10169,7 +10175,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>15</v>
@@ -10183,7 +10189,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>14</v>
@@ -10197,7 +10203,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>14</v>
@@ -10211,7 +10217,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>13</v>
@@ -10225,7 +10231,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>13</v>
@@ -10297,7 +10303,7 @@
         <v>70</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>14</v>
@@ -10376,7 +10382,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>20</v>
@@ -10388,7 +10394,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>40</v>
@@ -10402,7 +10408,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>40</v>
@@ -10416,7 +10422,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>40</v>
@@ -10472,7 +10478,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10480,7 +10486,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10629,7 +10635,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -10649,7 +10655,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -10663,7 +10669,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -10677,7 +10683,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -10691,7 +10697,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -10705,7 +10711,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -10719,7 +10725,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -10733,7 +10739,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -10887,7 +10893,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10895,7 +10901,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11044,7 +11050,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -11064,7 +11070,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -11078,7 +11084,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -11092,7 +11098,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -11106,7 +11112,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -11120,7 +11126,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -11134,7 +11140,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>37</v>
@@ -11148,7 +11154,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -11302,7 +11308,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11310,7 +11316,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11459,7 +11465,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>36</v>
@@ -11479,7 +11485,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>37</v>
@@ -11493,7 +11499,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>38</v>
@@ -11507,7 +11513,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>36</v>
@@ -11521,7 +11527,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>37</v>
@@ -11535,7 +11541,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -11549,7 +11555,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>39</v>
@@ -11563,7 +11569,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>39</v>
@@ -11717,7 +11723,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11725,7 +11731,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12583,7 +12589,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12591,7 +12597,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12950,7 +12956,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>35</v>
@@ -12964,7 +12970,7 @@
         <v>4</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>35</v>
@@ -12978,7 +12984,7 @@
         <v>1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>5</v>
@@ -13034,7 +13040,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13042,7 +13048,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13134,7 +13140,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -13174,7 +13180,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -13194,7 +13200,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -13386,7 +13392,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13394,7 +13400,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13486,7 +13492,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>20</v>
@@ -13526,7 +13532,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>30</v>
@@ -13546,7 +13552,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>30</v>
@@ -13738,7 +13744,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13746,7 +13752,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13835,7 +13841,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -13855,7 +13861,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -13943,7 +13949,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>38</v>
@@ -14153,7 +14159,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14161,7 +14167,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14262,7 +14268,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>40</v>
@@ -14291,7 +14297,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -14320,7 +14326,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -14378,7 +14384,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>38</v>
@@ -14406,7 +14412,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>42</v>
@@ -14420,7 +14426,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -14434,7 +14440,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>38</v>
@@ -14448,7 +14454,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>42</v>
@@ -14462,7 +14468,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>38</v>
@@ -14616,7 +14622,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14624,7 +14630,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14754,7 +14760,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>40</v>
@@ -14783,7 +14789,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>40</v>
@@ -14883,7 +14889,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>42</v>
@@ -14897,7 +14903,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>42</v>
@@ -14911,7 +14917,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>44</v>
@@ -14925,7 +14931,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>44</v>
@@ -15564,8 +15570,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L29" activeCellId="0" sqref="L29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
modify evolution mechanisms for many species
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="27"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="AbandonedShip_HiddenFloorCorr" sheetId="1" state="visible" r:id="rId2"/>
@@ -20821,8 +20821,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21083,7 +21083,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>22</v>
@@ -21111,7 +21111,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>24</v>
@@ -22494,7 +22494,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change more evolutions, adjust wild pokemon levels
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="23"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="AbandonedShip_HiddenFloorCorr" sheetId="1" state="visible" r:id="rId2"/>
@@ -16007,8 +16007,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16131,10 +16131,10 @@
         <v>23</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="0" t="n">
         <v>20</v>
@@ -16163,10 +16163,10 @@
         <v>38</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19505,7 +19505,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19806,10 +19806,10 @@
         <v>17</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>10</v>
@@ -19853,10 +19853,10 @@
         <v>12</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>20</v>
@@ -20821,7 +20821,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more modifications related to base battle engine upgrade
</commit_message>
<xml_diff>
--- a/wild_data/wild_data.xlsx
+++ b/wild_data/wild_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="70"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="122"/>
   </bookViews>
   <sheets>
     <sheet name="AbandonedShip_HiddenFloorCorr" sheetId="1" state="visible" r:id="rId2"/>
@@ -129,8 +129,8 @@
     <sheet name="SkyPillar_5F" sheetId="119" state="visible" r:id="rId120"/>
     <sheet name="SlateportCity" sheetId="120" state="visible" r:id="rId121"/>
     <sheet name="SootopolisCity" sheetId="121" state="visible" r:id="rId122"/>
-    <sheet name="Underwater1" sheetId="122" state="visible" r:id="rId123"/>
-    <sheet name="Underwater2" sheetId="123" state="visible" r:id="rId124"/>
+    <sheet name="Underwater_Route124" sheetId="122" state="visible" r:id="rId123"/>
+    <sheet name="Underwater_Route126" sheetId="123" state="visible" r:id="rId124"/>
     <sheet name="VictoryRoad_1F" sheetId="124" state="visible" r:id="rId125"/>
     <sheet name="VictoryRoad_B1F" sheetId="125" state="visible" r:id="rId126"/>
     <sheet name="VictoryRoad_B2F" sheetId="126" state="visible" r:id="rId127"/>
@@ -1374,10 +1374,10 @@
     <t xml:space="preserve">GYARADOS</t>
   </si>
   <si>
-    <t xml:space="preserve">MAP_UNDERWATER1</t>
+    <t xml:space="preserve">MAP_UNDERWATER_ROUTE124</t>
   </si>
   <si>
-    <t xml:space="preserve">gUnderwater1</t>
+    <t xml:space="preserve">gUnderwater_Route124</t>
   </si>
   <si>
     <t xml:space="preserve">CHINCHOU</t>
@@ -1386,10 +1386,10 @@
     <t xml:space="preserve">RELICANTH</t>
   </si>
   <si>
-    <t xml:space="preserve">MAP_UNDERWATER2</t>
+    <t xml:space="preserve">MAP_UNDERWATER_ROUTE126</t>
   </si>
   <si>
-    <t xml:space="preserve">gUnderwater2</t>
+    <t xml:space="preserve">gUnderwater_Route126</t>
   </si>
   <si>
     <t xml:space="preserve">MAP_VICTORY_ROAD_1F</t>
@@ -13455,7 +13455,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13806,8 +13806,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -43801,7 +43801,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>